<commit_message>
Update DOkumentation- bitte mal anschauen und Update Excel
</commit_message>
<xml_diff>
--- a/Meetings/Doku/Doku_Einteilung-Inhaltsverzeichnis.xlsx
+++ b/Meetings/Doku/Doku_Einteilung-Inhaltsverzeichnis.xlsx
@@ -11,13 +11,14 @@
     <sheet name="Planungsphase" sheetId="2" r:id="rId2"/>
     <sheet name="Durchführungsphase" sheetId="3" r:id="rId3"/>
     <sheet name="Abschlussphase" sheetId="4" r:id="rId4"/>
+    <sheet name="Skilltabelle" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="130">
   <si>
     <r>
       <t xml:space="preserve">Projektstart EinkaufsApp
@@ -1438,9 +1439,6 @@
 5. Ausgabe + weiter zum Einkauf</t>
   </si>
   <si>
-    <t>Planungsphase Designer</t>
-  </si>
-  <si>
     <t>Ideen/Vorschläge</t>
   </si>
   <si>
@@ -1507,6 +1505,168 @@
       <t xml:space="preserve">
 *Ablaufplan (s. Reiter "Ablaufplan"), nicht fix</t>
     </r>
+  </si>
+  <si>
+    <t>*Idee: Facebook, Twitter usw. zur Registrierung verwenden
+*Artikel zuweisen nach Einkauf auf Gruppenmitglieder (Noch muss gleich bei Einkauf eingepflegt werden)
+*was passiert falls kein Empfang (Offline-Version)</t>
+  </si>
+  <si>
+    <t>Ideen/Vorschläge
+Designer</t>
+  </si>
+  <si>
+    <t>Ideen/Vorschläge
+alle</t>
+  </si>
+  <si>
+    <t>ToDos</t>
+  </si>
+  <si>
+    <t>DB Modell überarbeitet, Arbeitspakete für jeden zugewiesen über Trello:
+Viktor Fuchs:
+Namenskonventionen ausarbeiten - Variablen und Funktionen
+Eric Sorgalla:
+Einführung in die Technik- Präsentation vorbereiten
+Modulplan erstellen
+Kanban-Board erstellen
+Florian Schmitt:
+HTML-Code der Proto.io App exportieren u. durchgehen
+Michael Hein:
+bereits erstellten Code kommentieren
+Sebastian Kiepsch:
+Einführung in die Technik- Präsentation vorbereiten
+Modulplan erstellen
+bereits erstellten Code kommentieren
+offene Aufgaben:
+*aktualisiertes DB Modell erstellen
+*EAN Kategorien recherchieren und Tabelle füllen
+*neues DB Modell implementieren
+*UML Diagramm erstellen</t>
+  </si>
+  <si>
+    <t>Planungsphase</t>
+  </si>
+  <si>
+    <t>*Gruppenverwaltung wurde zu Verwaltung allgemein:  Verwaltung von Gruppen UND KONTAKTE 
+*Kontaktverwaltung wird noch erstellt</t>
+  </si>
+  <si>
+    <t>Gespräch mit Frau Wieland + Herrn Georg</t>
+  </si>
+  <si>
+    <t>*Dozenten wollen GitHub Link für Repositories
+*Klassendiagramm: z.B. Kühlschrank mit Produkten und Verfallsdatum,…. --&gt; muss nur in Doku stehen!
+*Vorgehensmodell sollten wir nennen
+*Liste von Anforderungen an App ist sehr interessant für Frau Wieland, Anforderungen struturieren nach: basic, must have, nice to have und priorisieren
+*scope: Sicherheit!! ganz wichtig und unbedingt in Doku aufnehmen
+*out of focus Anforderungen sollen auch angegebenund priorisiert werden 
+*Architektur unbedingt angeben in Doku! Multi-Tier
+*Frameworks die genutzt werden, müssen gekennzeichnet werden
+*Frau Wieland hat Qualitätsmesser für Frameworks
+*private, package,protected sind in Ordnung aber public ist nicht gut
+Infos für Präsentation:
+*20min Zeit zum präsentieren, es kann auch nur einer oder zwei votragen
+*Video vorfühen ist in Ordnung
+*Fokus der Präsentation liegt auf Frau Wieland und NICHT auf Kunde!
+Infos für Doku:
+*ca. 30 Seiten als .pdf in ilias abzugeben
+*Handbuch und Installationsanweisung muss in den Anhang
+*alles was &gt;1 Tag Verspätung hat kostet Prozente!
+Termininfo:
+*08.01.2016: Vorstellung der Präsentation- Presse wird anwesend sein; frühestes Ende um 16 Uhr</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Team</t>
+  </si>
+  <si>
+    <t>Skills vor Projektstart</t>
+  </si>
+  <si>
+    <t>Skills nach Projektstart</t>
+  </si>
+  <si>
+    <t>Moritz Karsten</t>
+  </si>
+  <si>
+    <t>*  Zwei Jahre Projektansprechpartner Messe Berlin
+*  Application Management</t>
+  </si>
+  <si>
+    <t>Huong Dang</t>
+  </si>
+  <si>
+    <t>* Zwei Jahre Vertrieb
+* Tools LaTex
+* Grundlagen VBA</t>
+  </si>
+  <si>
+    <t>Markus Hube</t>
+  </si>
+  <si>
+    <t>Projektleiter</t>
+  </si>
+  <si>
+    <t>*    Zwei Jahre PMO der operational services
+*    Zwei Jahre Programmiererfahrung (VBA)
+*   Bereits Vorarbeit zum Thema geleistet</t>
+  </si>
+  <si>
+    <t>Annika Köstler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Zwei Jahre Controlling
+* Tools Latex
+*Grundkenntnisse VBA
+*Protokollierung von Meetings </t>
+  </si>
+  <si>
+    <t>Michael Hein</t>
+  </si>
+  <si>
+    <t>Entwicklung</t>
+  </si>
+  <si>
+    <t>* Zwei Jahre Applikations Administration
+* Java Erfahrung
+*VBA Erfahrung
+*Skript Programmierung</t>
+  </si>
+  <si>
+    <t>Moritz Schaub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* 2 Jahre Co-Product Owner in iOS und Android Messaging Produkt in AGILER Entwicklung (internationales, crossfunktionales Team)
+* Erstellung von komplexen Prototypen mit Proto.io auf Basis von HTML5
+* Vorbereitung, Durchführung von Design Thinking Workshops, Kundeninterviews mit Zielgruppen (anhand von Proto.io) , A/B Testing, Designstudien
+* Stakeholder Management 
+</t>
+  </si>
+  <si>
+    <t>Eric Sorgalla</t>
+  </si>
+  <si>
+    <t>*Grundkenntnisse (Java, C/C++,Javascript,HTML/CSS,VBA,SQL)
+*1 Jahr Projektleitung ISIPT (nur kaufmännische Verantwortung)</t>
+  </si>
+  <si>
+    <t>Jannis Grohs</t>
+  </si>
+  <si>
+    <t>*Datenbanken (MYSQL, Apex)
+*Programmiererfahrung (VBA, JAVA, Apex)
+*Projektmanagement
+*Design + Marketingtechniken</t>
+  </si>
+  <si>
+    <t>Victor Fuchs</t>
+  </si>
+  <si>
+    <t>*gute Excelkenntnisse
+*gute Kenntnisse RW/C</t>
   </si>
 </sst>
 </file>
@@ -1556,7 +1716,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1575,8 +1735,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1612,11 +1778,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1900,16 +2077,12 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1917,8 +2090,30 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -2223,7 +2418,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D14" sqref="A14:D14"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2417,17 +2612,17 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="108" t="s">
+      <c r="A14" s="106" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="109">
+      <c r="B14" s="107">
         <v>42304</v>
       </c>
       <c r="C14" s="100" t="s">
+        <v>95</v>
+      </c>
+      <c r="D14" s="105" t="s">
         <v>96</v>
-      </c>
-      <c r="D14" s="107" t="s">
-        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -2437,10 +2632,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView topLeftCell="A26" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2756,15 +2951,15 @@
     </row>
     <row r="19" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A19" s="69" t="s">
-        <v>95</v>
-      </c>
-      <c r="B19" s="106">
+        <v>94</v>
+      </c>
+      <c r="B19" s="99">
         <v>42303.540972222225</v>
       </c>
       <c r="C19" s="100" t="s">
         <v>71</v>
       </c>
-      <c r="D19" s="107" t="s">
+      <c r="D19" s="105" t="s">
         <v>72</v>
       </c>
     </row>
@@ -2772,7 +2967,7 @@
       <c r="A20" s="93" t="s">
         <v>75</v>
       </c>
-      <c r="B20" s="81">
+      <c r="B20" s="96">
         <v>42306</v>
       </c>
       <c r="C20" s="93" t="s">
@@ -2784,13 +2979,13 @@
     </row>
     <row r="21" spans="1:5" ht="405" x14ac:dyDescent="0.25">
       <c r="A21" s="93" t="s">
+        <v>98</v>
+      </c>
+      <c r="B21" s="96">
+        <v>42306</v>
+      </c>
+      <c r="C21" s="93" t="s">
         <v>85</v>
-      </c>
-      <c r="B21" s="81">
-        <v>42306</v>
-      </c>
-      <c r="C21" s="93" t="s">
-        <v>86</v>
       </c>
       <c r="D21" s="94" t="s">
         <v>84</v>
@@ -2798,32 +2993,75 @@
     </row>
     <row r="22" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A22" s="93" t="s">
-        <v>85</v>
-      </c>
-      <c r="B22" s="81">
+        <v>98</v>
+      </c>
+      <c r="B22" s="96">
         <v>42306</v>
       </c>
       <c r="C22" s="93" t="s">
+        <v>86</v>
+      </c>
+      <c r="D22" s="93" t="s">
         <v>87</v>
-      </c>
-      <c r="D22" s="93" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="93" t="s">
-        <v>94</v>
-      </c>
-      <c r="B23" s="103">
+        <v>93</v>
+      </c>
+      <c r="B23" s="109">
         <v>42307</v>
       </c>
-      <c r="C23" s="104" t="s">
+      <c r="C23" s="103" t="s">
+        <v>91</v>
+      </c>
+      <c r="D23" s="104" t="s">
         <v>92</v>
       </c>
-      <c r="D23" s="105" t="s">
+      <c r="E23" s="89"/>
+    </row>
+    <row r="24" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A24" s="93" t="s">
+        <v>99</v>
+      </c>
+      <c r="B24" s="96">
+        <v>42311</v>
+      </c>
+      <c r="C24" s="93" t="s">
+        <v>85</v>
+      </c>
+      <c r="D24" s="83" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="405" x14ac:dyDescent="0.25">
+      <c r="A25" s="93" t="s">
         <v>93</v>
       </c>
-      <c r="E23" s="89"/>
+      <c r="B25" s="92">
+        <v>42312</v>
+      </c>
+      <c r="C25" s="95" t="s">
+        <v>100</v>
+      </c>
+      <c r="D25" s="104" t="s">
+        <v>101</v>
+      </c>
+      <c r="E25" s="93"/>
+    </row>
+    <row r="26" spans="1:5" ht="375" x14ac:dyDescent="0.25">
+      <c r="A26" s="93" t="s">
+        <v>102</v>
+      </c>
+      <c r="B26" s="108">
+        <v>42313</v>
+      </c>
+      <c r="C26" s="112" t="s">
+        <v>104</v>
+      </c>
+      <c r="D26" s="94" t="s">
+        <v>105</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -2832,10 +3070,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2882,18 +3120,32 @@
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="95" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B3" s="99">
         <v>42303</v>
       </c>
       <c r="C3" s="100" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" s="101" t="s">
         <v>89</v>
       </c>
-      <c r="D3" s="101" t="s">
+      <c r="E3" s="102"/>
+    </row>
+    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="95" t="s">
         <v>90</v>
       </c>
-      <c r="E3" s="102"/>
+      <c r="B4" s="111">
+        <v>42312</v>
+      </c>
+      <c r="C4" s="63" t="s">
+        <v>88</v>
+      </c>
+      <c r="D4" s="110" t="s">
+        <v>103</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -2912,4 +3164,147 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.7109375" customWidth="1"/>
+    <col min="2" max="2" width="29.5703125" customWidth="1"/>
+    <col min="3" max="3" width="34.7109375" customWidth="1"/>
+    <col min="4" max="4" width="28.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="113" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="113" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" s="114" t="s">
+        <v>108</v>
+      </c>
+      <c r="D1" s="115" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="45" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" s="45" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="66" t="s">
+        <v>111</v>
+      </c>
+      <c r="D2" s="89"/>
+    </row>
+    <row r="3" spans="1:4" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="45" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="66" t="s">
+        <v>113</v>
+      </c>
+      <c r="D3" s="89"/>
+    </row>
+    <row r="4" spans="1:4" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="45" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" s="45" t="s">
+        <v>115</v>
+      </c>
+      <c r="C4" s="66" t="s">
+        <v>116</v>
+      </c>
+      <c r="D4" s="89"/>
+    </row>
+    <row r="5" spans="1:4" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="45" t="s">
+        <v>117</v>
+      </c>
+      <c r="B5" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="66" t="s">
+        <v>118</v>
+      </c>
+      <c r="D5" s="89"/>
+    </row>
+    <row r="6" spans="1:4" ht="133.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="45" t="s">
+        <v>119</v>
+      </c>
+      <c r="B6" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="C6" s="66" t="s">
+        <v>121</v>
+      </c>
+      <c r="D6" s="89"/>
+    </row>
+    <row r="7" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="45" t="s">
+        <v>122</v>
+      </c>
+      <c r="B7" s="45" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="66" t="s">
+        <v>123</v>
+      </c>
+      <c r="D7" s="89"/>
+    </row>
+    <row r="8" spans="1:4" ht="141.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="45" t="s">
+        <v>124</v>
+      </c>
+      <c r="B8" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="C8" s="66" t="s">
+        <v>125</v>
+      </c>
+      <c r="D8" s="89"/>
+    </row>
+    <row r="9" spans="1:4" ht="132" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="45" t="s">
+        <v>126</v>
+      </c>
+      <c r="B9" s="45" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="66" t="s">
+        <v>127</v>
+      </c>
+      <c r="D9" s="89"/>
+    </row>
+    <row r="10" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A10" s="45" t="s">
+        <v>128</v>
+      </c>
+      <c r="B10" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="C10" s="66" t="s">
+        <v>129</v>
+      </c>
+      <c r="D10" s="89"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>